<commit_message>
Revert "updated external-debugger Vplan"
This reverts commit a332ec0cad74a85d1ad794b521847a5978a67ee4.
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/debug-trace/CV32E40P_external-debugger.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/debug-trace/CV32E40P_external-debugger.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/Verification/v2_VerifPlans/Simulation/debug-trace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aherrera\Documents\4_OSHW_Design&amp;Verif_40%\4_Debug-Trace_VerfiComponent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6518D73E-6ED0-4CBD-9613-09300D8E3CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA70C333-A5AD-4048-90F6-0D063586A217}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6518D73E-6ED0-4CBD-9613-09300D8E3CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3705" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="345" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="External-Debugger" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'External-Debugger'!$A$1:$J$18</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,24 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={2C6072FB-E9E5-40E1-A43B-E7C2E11EE31C}</author>
-  </authors>
-  <commentList>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{2C6072FB-E9E5-40E1-A43B-E7C2E11EE31C}">
-      <text>
-        <t>[Commentaire à thread]
-Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
-Commentaire :
-    Already descrbied in CV32E40P_debug.xlsx</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
   <si>
@@ -563,6 +545,31 @@
     <t>Self-checking of DSCRATCH registers expected values while in Debug-Mode.</t>
   </si>
   <si>
+    <r>
+      <t>Debugger single steps a instruction and re-enters Debug-Mode by setting step bit (DCSR[2]) before setting "resumereq" in Debug Module</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if implemented</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.
+Interrupts can be enaled or disabled during stepping by setting the stepi bit in the DCSR</t>
+    </r>
+  </si>
+  <si>
     <t>Self-checking of DPC and PC against three expected values: before stepping; during each step; and after exiting Debug-Mode</t>
   </si>
   <si>
@@ -578,40 +585,13 @@
   </si>
   <si>
     <t>Not yet coded</t>
-  </si>
-  <si>
-    <r>
-      <t>Debugger single steps a instruction and re-enters Debug-Mode by setting step bit (DCSR[2]) before setting "resumereq" in Debug Module</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> if implemented</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.
-Interrupts can be enaled or disabled during stepping by setting the stepi bit in the DCSR</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -635,21 +615,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -782,24 +747,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -807,20 +779,35 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -832,6 +819,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -839,83 +829,74 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,14 +986,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Xavier Aubert" id="{101A2A43-5A74-4A70-A99B-E5EFFF368335}" userId="S::xavier.aubert@dolphin.fr::db9aa7a3-bc41-42e8-89c7-c757ca35a621" providerId="AD"/>
-</personList>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1306,43 +1281,35 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A18" dT="2023-01-30T16:39:32.34" personId="{101A2A43-5A74-4A70-A99B-E5EFFF368335}" id="{2C6072FB-E9E5-40E1-A43B-E7C2E11EE31C}">
-    <text>Already descrbied in CV32E40P_debug.xlsx</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF2E75B6"/>
   </sheetPr>
   <dimension ref="A1:AMI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="49.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="4" customWidth="1"/>
-    <col min="11" max="1023" width="8.7109375" style="6"/>
-    <col min="1024" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="24.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" style="7" customWidth="1"/>
+    <col min="11" max="1023" width="8.6640625" style="8"/>
+    <col min="1024" max="16384" width="8.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1374,20 +1341,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1397,29 +1364,29 @@
         <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="51" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="J2" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1429,121 +1396,121 @@
         <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="51" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="J3" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="12" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="I4" s="51" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="J4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="37" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="I5" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="J5" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="J6" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1553,140 +1520,140 @@
         <v>49</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="I7" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="J7" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="33" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="34" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="I8" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="134.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="J8" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="31"/>
+      <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="35"/>
       <c r="H9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="J9" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="11" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="J10" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>66</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="I11" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="J11" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="24" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="39" t="s">
@@ -1698,47 +1665,47 @@
       <c r="G12" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="30" t="s">
+      <c r="H12" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="I12" s="49" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="J12" s="50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="28" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="27"/>
-    </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="H13" s="47"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50"/>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="24" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="40"/>
@@ -1748,47 +1715,47 @@
       <c r="G14" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="30" t="s">
+      <c r="H14" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="I14" s="49" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="J14" s="50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="45"/>
       <c r="G15" s="45"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="27"/>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="H15" s="47"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E16" s="40"/>
@@ -1798,68 +1765,68 @@
       <c r="G16" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="30" t="s">
+      <c r="H16" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="I16" s="49" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="J16" s="50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="28" t="s">
         <v>70</v>
       </c>
       <c r="E17" s="41"/>
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="27"/>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="H17" s="47"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+    </row>
+    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1870,7 +1837,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1885,16 +1852,6 @@
   </sheetData>
   <autoFilter ref="A1:J18" xr:uid="{B0FCC5CC-B046-4807-9594-8537D0CA2801}"/>
   <mergeCells count="19">
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="J16:J17"/>
@@ -1904,276 +1861,18 @@
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6f429ff05de3a495de36a912eeee1367">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dba9ee4a9862521e056f2186065b8ec" ns2:_="" ns3:_="">
-    <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <xsd:import namespace="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68bd86b6-d639-4884-9680-62e746fab3da" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="21" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="51aa521f-7cbd-47c5-afee-4a8147a04eed" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{67132edb-7ad2-4046-b569-46a3488a100c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="51aa521f-7cbd-47c5-afee-4a8147a04eed">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C475241-7082-45E6-975B-719FEF39FAE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BB0904E-9F2F-4B3E-A921-09F7ABEC6C17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>